<commit_message>
Gjort integrationstester 2, 4, 7, 8, 9 och lagt i "integrationstester" mapp- Varanamn godtar "@" - need fix!
Gjort integrationstester 2, 4, 7, 8, 9 och lagt i "integrationstester"
mapp- Varanamn godtar "@" - need fix!

Uppdaterade även Excellen med de ekvivalensklasser vi lade till - vet
dock inte exakt hur det ska göras med "T22" - vad det ska vara för
input?
</commit_message>
<xml_diff>
--- a/Dokumentation/Ekvivalensklasser.xlsx
+++ b/Dokumentation/Ekvivalensklasser.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Skola\INTE\Git\INTEGrupp7\Dokumentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="147">
   <si>
     <t>Ekvivalensklass</t>
   </si>
@@ -258,30 +263,15 @@
     <t>T5</t>
   </si>
   <si>
-    <t>V1, V3, V8, V14, VA1, VA6, E2, E3, E5, E7, R1, R4</t>
-  </si>
-  <si>
     <t>12, dollar, Kg, Äpplen, 1234567891234, 8.51, 123, timestamp, 24, 13, Pensionär, 10%</t>
   </si>
   <si>
     <t>5, styck, Sudd, 1234567890123, euro, 9.39, 12345, timestamp, 23,</t>
   </si>
   <si>
-    <t>V1, V4, V8, V15, VA2, VA6, E2, E3, E5, E7,</t>
-  </si>
-  <si>
     <t>16, liter, Mjölk, 9876543210987, sek, 1, 567, timestamp, 27, 4</t>
   </si>
   <si>
-    <t>V1, V5, V8, V14, VA3, VA6, E2, E3, E5, E7,</t>
-  </si>
-  <si>
-    <t>V1, V8, V10, V15, VA1, VA6, E2, E3, E5, E7,</t>
-  </si>
-  <si>
-    <t>V1, V8, V11, V14, VA2, VA6, E2, E3, E5, E7,</t>
-  </si>
-  <si>
     <t>18, saffran, gram, 2345678901111, dollar, 9.13, 987, timestamp, 19.95, 1,</t>
   </si>
   <si>
@@ -339,9 +329,6 @@
     <t>Vara pris&gt;=1,Valuta namn dollar, Testa enhet KG, Testa namn, Streckkod=13 siffror  Valuta kurs &gt;0, Kvittonummer &gt; 0 siffror, Tid=nuvarande tid, Totalpris&gt;0, Antal&gt;0, Rabattnamn, Rabattvärde&gt;0</t>
   </si>
   <si>
-    <t>Vara pris&gt;=1, Vara enhet styck, Varunamn A-Ö,  Streckkod=13 siffror Valuta namn euro, Valuta kurs&gt;0, Kvittonummer&gt; 0siffror, Tid=nuvarande tid, Totalpris&gt;0</t>
-  </si>
-  <si>
     <t>Vara pris&gt;=1, Vara enhet liter, Varunamn A-Ö, Streckkod=13 siffror Valutanamn sek, Valuta kurs&gt;0, Kvittonummer &gt;0 siffror, Tid=nuvarande tid, Totalpris&gt;0, Antal&gt;0,</t>
   </si>
   <si>
@@ -424,13 +411,64 @@
   </si>
   <si>
     <t>12, dollar, Kg, Äpplen, 1234567891234, 8.51, 123, timestamp, 24, 13, Pensionär, 110%</t>
+  </si>
+  <si>
+    <t>KR1</t>
+  </si>
+  <si>
+    <t>antal av vara &lt;1</t>
+  </si>
+  <si>
+    <t>KR2</t>
+  </si>
+  <si>
+    <t>antal av vara &gt;=1</t>
+  </si>
+  <si>
+    <t>Vara pris&gt;=1, Vara enhet styck, Varunamn A-Ö,  Streckkod=13 siffror Valuta namn euro, Valuta kurs&gt;0, Kvittonummer&gt; 0siffror, Tid=nuvarande tid, Antal&gt;0</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>kvittorader&lt;1</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>kvittorader&gt;=1</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>Kvittorader&lt;1</t>
+  </si>
+  <si>
+    <t>V1, V3, V8, V14, VA1, VA6, E2, E3, E5, E7, R1, R4, E10</t>
+  </si>
+  <si>
+    <t>V1, V4, V8, V15, VA2, VA6, E2, E3, E5, E7, E10</t>
+  </si>
+  <si>
+    <t>V1, V5, V8, V14, VA3, VA6, E2, E3, E5, E7, E10</t>
+  </si>
+  <si>
+    <t>V1, V8, V10, V15, VA1, VA6, E2, E3, E5, E7, E10</t>
+  </si>
+  <si>
+    <t>V1, V8, V11, V14, VA2, VA6, E2, E3, E5, E7, E10</t>
+  </si>
+  <si>
+    <t>Kvitto(987, null) (?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,16 +549,14 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -540,11 +576,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,7 +645,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,9 +677,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -671,6 +712,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -846,23 +888,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="171.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="208.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>32</v>
       </c>
@@ -879,7 +921,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -895,7 +937,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -909,7 +951,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -923,7 +965,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -937,7 +979,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
@@ -951,7 +993,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
@@ -963,7 +1005,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -975,7 +1017,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -990,7 +1032,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
@@ -1002,7 +1044,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1016,7 +1058,7 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>58</v>
       </c>
@@ -1030,31 +1072,31 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="3"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="3"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>61</v>
       </c>
@@ -1068,7 +1110,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
@@ -1080,7 +1122,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="4"/>
@@ -1088,7 +1130,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>32</v>
       </c>
@@ -1104,7 +1146,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75">
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -1118,7 +1160,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
@@ -1132,7 +1174,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -1146,7 +1188,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75">
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -1158,24 +1200,24 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="3"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1184,7 +1226,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="4"/>
@@ -1192,7 +1234,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>32</v>
       </c>
@@ -1208,7 +1250,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
@@ -1220,7 +1262,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
@@ -1234,7 +1276,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>65</v>
       </c>
@@ -1248,7 +1290,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -1260,7 +1302,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>67</v>
       </c>
@@ -1274,7 +1316,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>68</v>
       </c>
@@ -1286,7 +1328,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>69</v>
       </c>
@@ -1300,7 +1342,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>70</v>
       </c>
@@ -1312,566 +1354,612 @@
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="C35" s="5"/>
       <c r="D35" s="3"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C38" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="3"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="3"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="3"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="2" t="s">
+      <c r="C50" s="5"/>
+      <c r="D50" s="3"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="2" t="s">
+      <c r="D51" s="3"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" s="1" customFormat="1">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42" s="11"/>
-      <c r="F42"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="9" t="s">
+      <c r="C52" s="5"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53" s="11"/>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B54" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C54" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D54" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E54" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F54" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="14" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B55" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" s="14"/>
+      <c r="F55" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="14"/>
+      <c r="F56" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="14"/>
+      <c r="F57" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="14"/>
+      <c r="F58" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="14"/>
+      <c r="F59" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" s="14"/>
+      <c r="F60" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="14"/>
+      <c r="F61" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="14" t="s">
+      <c r="D64" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="15"/>
-      <c r="F45" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="14" t="s">
+      <c r="D65" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B48" s="14" t="s">
+      <c r="D66" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="B67" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D67" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E51" s="15"/>
-      <c r="F51" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53" s="15" t="s">
+      <c r="E67" s="14"/>
+      <c r="F67" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="B68" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="14" t="s">
+      <c r="B69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D54" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="14" t="s">
+      <c r="B70" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="14" t="s">
+      <c r="B72" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B56" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="14" t="s">
+      <c r="B73" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" s="16" t="s">
+      <c r="B74" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D57" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="14" t="s">
+      <c r="D74" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B58" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="14" t="s">
+      <c r="B75" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15" t="s">
+      <c r="D75" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="17"/>
-      <c r="D65" s="13"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="17"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="17"/>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="17"/>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="17"/>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="17"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="17"/>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>146</v>
+      </c>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="4:4">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="4:4">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="4:4">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="4:4">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="4:4">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="3"/>
     </row>
   </sheetData>
@@ -1881,24 +1969,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Glömde lägga till var de nya ekv. klasserna testas
</commit_message>
<xml_diff>
--- a/Dokumentation/Ekvivalensklasser.xlsx
+++ b/Dokumentation/Ekvivalensklasser.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="147">
   <si>
     <t>Ekvivalensklass</t>
   </si>
@@ -892,7 +892,7 @@
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,7 +1933,12 @@
       <c r="C76" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D76" s="3"/>
+      <c r="D76" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D77" s="3"/>

</xml_diff>